<commit_message>
1. Query start/end optional 2. update tidy report format
</commit_message>
<xml_diff>
--- a/report_template/tidyReport.xlsx
+++ b/report_template/tidyReport.xlsx
@@ -24,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>整理課報表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>流動卡代號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>工作</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,6 +67,18 @@
   </si>
   <si>
     <t>開始:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流動卡號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>訂單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>品名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -459,19 +467,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="4" width="9.875" customWidth="1"/>
+    <col min="5" max="5" width="6.25" customWidth="1"/>
+    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="7" max="7" width="5.125" customWidth="1"/>
+    <col min="8" max="8" width="4.75" customWidth="1"/>
+    <col min="9" max="9" width="5.375" customWidth="1"/>
+    <col min="10" max="10" width="7.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -484,41 +499,47 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. finish date 2. export report
</commit_message>
<xml_diff>
--- a/report_template/tidyReport.xlsx
+++ b/report_template/tidyReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webApp\tights\report_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEB5A40-8537-42FF-9C8A-524FD3B81EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920CECDD-FE55-44CB-96A0-08CA98195DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>整理課報表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +96,14 @@
   </si>
   <si>
     <t>定型日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>結束日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>輸入日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -495,25 +503,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="12.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="4.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="1" max="10" width="12.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.75" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7.375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -531,66 +539,76 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>